<commit_message>
Got a decent result using the catagory -> regression attempt
</commit_message>
<xml_diff>
--- a/data/csv/api.xlsx
+++ b/data/csv/api.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanyohnk/Dropbox/dev/baseball/data/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1FB7234A-D5E9-0C4E-A871-DDC3F9B68C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95F113A-C4DD-6A44-B3AF-BC079ECF8CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17240"/>
+    <workbookView xWindow="40940" yWindow="-4260" windowWidth="28040" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="api" sheetId="1" r:id="rId1"/>
@@ -2941,7 +2941,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3776,13 +3776,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N916"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A830" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H847" sqref="H847"/>
+      <pane ySplit="1" topLeftCell="A826" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B854" sqref="B854:B855"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3836,7 +3836,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3900,7 +3900,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -4052,7 +4052,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -8502,7 +8502,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>177</v>
       </c>
@@ -8516,7 +8516,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>177</v>
       </c>
@@ -8530,7 +8530,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>177</v>
       </c>
@@ -8544,7 +8544,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>177</v>
       </c>
@@ -8567,7 +8567,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>177</v>
       </c>
@@ -8590,7 +8590,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>177</v>
       </c>
@@ -8616,7 +8616,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>177</v>
       </c>
@@ -8654,7 +8654,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>177</v>
       </c>
@@ -8692,7 +8692,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>177</v>
       </c>
@@ -8730,7 +8730,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>177</v>
       </c>
@@ -8768,7 +8768,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>177</v>
       </c>
@@ -8809,7 +8809,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>177</v>
       </c>
@@ -8847,7 +8847,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>177</v>
       </c>
@@ -28814,7 +28814,7 @@
         <v>4.2796532005164999E-2</v>
       </c>
     </row>
-    <row r="685" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="685" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A685" t="s">
         <v>838</v>
       </c>
@@ -28837,7 +28837,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="686" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="686" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A686" t="s">
         <v>838</v>
       </c>
@@ -28860,7 +28860,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="687" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="687" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A687" t="s">
         <v>838</v>
       </c>
@@ -28898,7 +28898,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="688" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="688" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A688" t="s">
         <v>838</v>
       </c>
@@ -28924,7 +28924,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="689" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="689" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A689" t="s">
         <v>838</v>
       </c>
@@ -28950,7 +28950,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="690" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="690" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A690" t="s">
         <v>838</v>
       </c>
@@ -28976,7 +28976,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="691" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="691" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A691" t="s">
         <v>838</v>
       </c>
@@ -29014,7 +29014,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="692" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="692" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A692" t="s">
         <v>838</v>
       </c>
@@ -29052,7 +29052,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="693" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="693" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A693" t="s">
         <v>838</v>
       </c>
@@ -29090,7 +29090,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="694" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="694" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A694" t="s">
         <v>838</v>
       </c>
@@ -29128,7 +29128,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="695" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="695" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A695" t="s">
         <v>838</v>
       </c>
@@ -29166,7 +29166,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="696" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="696" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A696" t="s">
         <v>838</v>
       </c>
@@ -29195,7 +29195,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="697" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="697" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A697" t="s">
         <v>838</v>
       </c>
@@ -29221,7 +29221,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="698" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="698" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A698" t="s">
         <v>838</v>
       </c>
@@ -29259,7 +29259,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="699" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="699" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A699" t="s">
         <v>838</v>
       </c>
@@ -29297,7 +29297,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="700" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="700" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A700" t="s">
         <v>838</v>
       </c>
@@ -29335,7 +29335,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="701" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="701" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A701" t="s">
         <v>838</v>
       </c>
@@ -29373,7 +29373,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="702" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="702" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A702" t="s">
         <v>838</v>
       </c>
@@ -29411,7 +29411,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="703" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="703" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A703" t="s">
         <v>838</v>
       </c>
@@ -29449,7 +29449,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="704" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="704" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A704" t="s">
         <v>838</v>
       </c>
@@ -29487,7 +29487,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="705" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="705" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A705" t="s">
         <v>838</v>
       </c>
@@ -29525,7 +29525,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="706" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="706" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A706" t="s">
         <v>838</v>
       </c>
@@ -29563,7 +29563,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="707" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="707" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A707" t="s">
         <v>838</v>
       </c>
@@ -33354,7 +33354,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="822" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="822" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A822" t="s">
         <v>939</v>
       </c>
@@ -33368,7 +33368,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="823" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="823" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A823" t="s">
         <v>939</v>
       </c>
@@ -33382,7 +33382,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="824" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="824" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A824" t="s">
         <v>939</v>
       </c>
@@ -33740,7 +33740,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="835" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="835" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A835" t="s">
         <v>939</v>
       </c>
@@ -33784,7 +33784,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="836" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="836" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A836" t="s">
         <v>939</v>
       </c>
@@ -33828,7 +33828,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="837" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="837" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A837" t="s">
         <v>939</v>
       </c>
@@ -33872,7 +33872,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="838" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="838" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A838" t="s">
         <v>939</v>
       </c>
@@ -34833,7 +34833,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="864" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="864" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A864" t="s">
         <v>939</v>
       </c>
@@ -34877,7 +34877,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="865" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="865" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A865" t="s">
         <v>939</v>
       </c>
@@ -34962,7 +34962,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="867" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="867" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A867" t="s">
         <v>939</v>
       </c>
@@ -36965,13 +36965,20 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N916">
+  <autoFilter ref="A1:N916" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="statcast_pitcher"/>
-        <filter val="statcast_pitcher_active_spin"/>
-        <filter val="statcast_pitcher_percentile_ranks"/>
-        <filter val="statcast_pitcher_pitch_movement"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="10">
+      <filters>
+        <filter val="2000"/>
+        <filter val="2004"/>
+        <filter val="2006"/>
+        <filter val="2008"/>
+        <filter val="2015"/>
+        <filter val="2016"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>